<commit_message>
Update package-functions.R and .Rmd
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackl\Documents\GitHub\LinearModel-RViz-Summer2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2AC34C-3B0F-4109-99E5-5BDE4B89BC78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59874AD8-910E-4EAB-84C2-CB5B76F31D21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="6" xr2:uid="{52C7A5B5-E4C9-488F-9EF2-517115249B59}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" firstSheet="3" activeTab="7" xr2:uid="{52C7A5B5-E4C9-488F-9EF2-517115249B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Week of 6-24 " sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="Week of 7-22" sheetId="5" r:id="rId5"/>
     <sheet name="Week of 8-5" sheetId="6" r:id="rId6"/>
     <sheet name="Week of 8-12" sheetId="7" r:id="rId7"/>
+    <sheet name="Week of 8-19" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Downloaded and setup GithubDesktop. Began reading on Git, GitHub, and Rprojects</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Added ability to not input cat variable. Worked on vignette and pkgdown.</t>
+  </si>
+  <si>
+    <t>Worked on documentation pages.</t>
+  </si>
+  <si>
+    <t>Dr. Ottosen's talk.</t>
   </si>
 </sst>
 </file>
@@ -1761,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B016F38F-B106-4526-BE73-F46877E66271}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,4 +1990,199 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3333C6-6938-4D2B-90FF-AB013823D652}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2-A2</f>
+        <v>0.12013888888888902</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43698</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4">
+        <f>C2</f>
+        <v>0.12013888888888902</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="C4" s="14">
+        <f>B4-A4</f>
+        <v>0.10763888888888895</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43699</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>0.83194444444444438</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8">
+        <f>B5-A5</f>
+        <v>-0.83194444444444438</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11">
+        <f>C4+C5</f>
+        <v>-0.72430555555555542</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8">
+        <f>B7-A7</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8">
+        <f>B9-A9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8">
+        <f>C9</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14">
+        <f>B11-A11</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11">
+        <f>C11</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8">
+        <f>B13-A13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8">
+        <f>C13</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="17">
+        <f>C3+C6+C8+C10+C12</f>
+        <v>-0.60416666666666641</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>